<commit_message>
Tambahan wira usaha tmpt & tanggal survey serta, bpkb atas nama untuk 2 w & 4 w dahsyat
</commit_message>
<xml_diff>
--- a/Parameter data Excel/Form Pemohon.xlsx
+++ b/Parameter data Excel/Form Pemohon.xlsx
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="152">
   <si>
     <t>NIK</t>
   </si>
@@ -490,6 +490,30 @@
   </si>
   <si>
     <t>New Bike</t>
+  </si>
+  <si>
+    <t>BPKB Atas nama</t>
+  </si>
+  <si>
+    <t>ATAS NAMA ORANG LAIN</t>
+  </si>
+  <si>
+    <t>Dahsyat - Multipurpose 4W</t>
+  </si>
+  <si>
+    <t>CALL CENTER</t>
+  </si>
+  <si>
+    <t>Jam Survey Tmpt usaha</t>
+  </si>
+  <si>
+    <t>Tanggal Survey usaha</t>
+  </si>
+  <si>
+    <t>Atas Nama Orang Lain (dalam 1 KK)</t>
+  </si>
+  <si>
+    <t>ATAS NAMA SENDIRI ( DEBITUR  PASANGAN )</t>
   </si>
 </sst>
 </file>
@@ -498,7 +522,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="166" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -565,7 +589,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma [0]" xfId="1" builtinId="6"/>
@@ -847,11 +871,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AM6"/>
+  <dimension ref="A1:AP6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="H5" sqref="H5"/>
+      <pane xSplit="2" topLeftCell="AJ1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AN3" sqref="AN3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -895,9 +919,12 @@
     <col min="37" max="37" width="12.7265625" bestFit="1" customWidth="1"/>
     <col min="38" max="38" width="10.08984375" bestFit="1" customWidth="1"/>
     <col min="39" max="39" width="13.26953125" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="43.453125" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="20.54296875" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="18.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
         <v>6</v>
       </c>
@@ -1015,8 +1042,17 @@
       <c r="AM1" t="s">
         <v>138</v>
       </c>
+      <c r="AN1" t="s">
+        <v>144</v>
+      </c>
+      <c r="AO1" t="s">
+        <v>148</v>
+      </c>
+      <c r="AP1" t="s">
+        <v>149</v>
+      </c>
     </row>
-    <row r="2" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
         <v>8</v>
       </c>
@@ -1135,8 +1171,17 @@
       <c r="AM2" s="3" t="s">
         <v>139</v>
       </c>
+      <c r="AN2" t="s">
+        <v>145</v>
+      </c>
+      <c r="AO2" s="8" t="s">
+        <v>133</v>
+      </c>
+      <c r="AP2" s="3" t="s">
+        <v>139</v>
+      </c>
     </row>
-    <row r="3" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
         <v>7</v>
       </c>
@@ -1216,10 +1261,10 @@
         <v>105</v>
       </c>
       <c r="AA3" t="s">
-        <v>119</v>
+        <v>146</v>
       </c>
       <c r="AB3" t="s">
-        <v>109</v>
+        <v>147</v>
       </c>
       <c r="AC3" t="s">
         <v>113</v>
@@ -1241,7 +1286,7 @@
         <v>13</v>
       </c>
       <c r="AI3" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="AJ3" t="s">
         <v>142</v>
@@ -1255,8 +1300,17 @@
       <c r="AM3" s="3" t="s">
         <v>141</v>
       </c>
+      <c r="AN3" t="s">
+        <v>150</v>
+      </c>
+      <c r="AO3" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="AP3" s="3" t="s">
+        <v>141</v>
+      </c>
     </row>
-    <row r="4" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A4" s="5" t="s">
         <v>8</v>
       </c>
@@ -1375,8 +1429,17 @@
       <c r="AM4" s="3" t="s">
         <v>140</v>
       </c>
+      <c r="AN4" t="s">
+        <v>151</v>
+      </c>
+      <c r="AO4" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="AP4" s="3" t="s">
+        <v>140</v>
+      </c>
     </row>
-    <row r="5" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="s">
         <v>8</v>
       </c>
@@ -1495,8 +1558,14 @@
       <c r="AM5" s="3" t="s">
         <v>139</v>
       </c>
+      <c r="AO5" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="AP5" s="3" t="s">
+        <v>139</v>
+      </c>
     </row>
-    <row r="6" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="s">
         <v>8</v>
       </c>
@@ -1613,6 +1682,12 @@
         <v>137</v>
       </c>
       <c r="AM6" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="AO6" s="8" t="s">
+        <v>137</v>
+      </c>
+      <c r="AP6" s="3" t="s">
         <v>139</v>
       </c>
     </row>

</xml_diff>